<commit_message>
part one mess files
</commit_message>
<xml_diff>
--- a/Measurement_Results/DLS/SmallPartData.xlsx
+++ b/Measurement_Results/DLS/SmallPartData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LIesDeceuninck/Bachelorproef2/Measurement_Results/DLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lies/Documents/Bachelorproef/Measurement_Results/DLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,11 +14,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -119,6 +119,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="M2" t="str">
+            <v>sigma</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="M24">
+            <v>3.0815531798104665</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,7 +411,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,13 +635,13 @@
         <f>AVERAGE(B13:I13)</f>
         <v>68.703749999999999</v>
       </c>
-      <c r="M13">
-        <f>_xlfn.VAR.P(B13:I13)</f>
-        <v>63.899398437499258</v>
-      </c>
-      <c r="N13">
-        <f>SQRT(M13)</f>
-        <v>7.9937099295320477</v>
+      <c r="M13" t="e">
+        <f ca="1">VAR.P+[1]Sheet1!$M$2+[1]Sheet1!$M$24(B13:I13)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N13" t="e">
+        <f ca="1">SQRT(M13)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>